<commit_message>
Adding colors to binary classifier
</commit_message>
<xml_diff>
--- a/HSPI.xlsx
+++ b/HSPI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Google Drive\לימודים\PHD\שברי ירך\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,12 +40,66 @@
         </r>
       </text>
     </comment>
+    <comment ref="AB3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Red</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = Low confidence.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Green</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = High confidence.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The color of this cell aplies also to the cell on the right.
+See paper for details.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Coefficient mFIM effectiveness</t>
   </si>
@@ -222,13 +276,19 @@
   </si>
   <si>
     <t>Days from surgery to rehabilitation</t>
+  </si>
+  <si>
+    <t>High safe</t>
+  </si>
+  <si>
+    <t>Low safe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -303,6 +363,18 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -606,7 +678,88 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -892,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1151,13 +1304,62 @@
     <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <conditionalFormatting sqref="Z2:AA2">
-    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(Z2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="between" id="{1C7B05F5-DAD0-4145-B872-721A357E3EDD}">
+            <xm:f>'Model params'!$C$33</xm:f>
+            <xm:f>'Model params'!$C$34</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThan" id="{3BF28A4E-D496-45FC-B7EA-9536FC3D7942}">
+            <xm:f>'Model params'!$C$34</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{267AFB30-92C3-4ADA-9B3A-D248AE64F8C8}">
+            <xm:f>'Model params'!$C$33</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AB3</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1399,10 +1601,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1797,8 +1999,24 @@
         <v>0.14562207995873369</v>
       </c>
     </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34">
+        <f>1-C33</f>
+        <v>0.77</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>